<commit_message>
updated - took off cracked positions
</commit_message>
<xml_diff>
--- a/Task3/Data/Raw_data/Electric_Anisotropy_&_Magnetic_Permeability_Data.xlsx
+++ b/Task3/Data/Raw_data/Electric_Anisotropy_&_Magnetic_Permeability_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saad J\Desktop\epri\myepri\Task3\Data\Raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saad J\Desktop\epri\Oct20_EPRI\Task3\Data\Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6C8382-1B0C-48BC-A611-718E65DD1A90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F677E9A-8ECC-437D-BF16-30F50CED4B4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" tabRatio="865" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" tabRatio="865" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="specimens" sheetId="7" r:id="rId1"/>
@@ -1834,16 +1834,13 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1852,13 +1849,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1882,6 +1882,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1891,19 +1897,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1918,28 +1921,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1949,6 +1937,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1979,21 +1994,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -20561,12 +20561,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="277" t="s">
+      <c r="A1" s="282" t="s">
         <v>113</v>
       </c>
       <c r="B1" s="278"/>
       <c r="C1" s="278"/>
-      <c r="D1" s="279"/>
+      <c r="D1" s="283"/>
       <c r="E1" s="174"/>
       <c r="F1" s="174"/>
       <c r="G1" s="174"/>
@@ -20574,12 +20574,12 @@
       <c r="I1" s="174"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="280" t="s">
+      <c r="A2" s="279" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="281"/>
-      <c r="C2" s="281"/>
-      <c r="D2" s="282"/>
+      <c r="B2" s="280"/>
+      <c r="C2" s="280"/>
+      <c r="D2" s="284"/>
       <c r="E2" s="174"/>
       <c r="F2" s="174"/>
       <c r="G2" s="183"/>
@@ -20588,14 +20588,14 @@
       <c r="J2" s="161"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="277" t="s">
+      <c r="A3" s="282" t="s">
         <v>145</v>
       </c>
       <c r="B3" s="278"/>
       <c r="C3" s="278" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="279"/>
+      <c r="D3" s="283"/>
       <c r="E3" s="174"/>
       <c r="F3" s="174"/>
       <c r="G3" s="183"/>
@@ -20604,27 +20604,27 @@
       <c r="J3" s="161"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="280" t="s">
+      <c r="A4" s="279" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="281"/>
-      <c r="C4" s="281" t="s">
+      <c r="B4" s="280"/>
+      <c r="C4" s="280" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="282"/>
+      <c r="D4" s="284"/>
       <c r="E4" s="174"/>
       <c r="F4" s="174"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
+      <c r="G4" s="281"/>
+      <c r="H4" s="281"/>
       <c r="I4" s="182"/>
       <c r="J4" s="161"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="283" t="s">
+      <c r="A5" s="276" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="284"/>
-      <c r="C5" s="284" t="s">
+      <c r="B5" s="277"/>
+      <c r="C5" s="277" t="s">
         <v>112</v>
       </c>
       <c r="D5" s="285"/>
@@ -20647,12 +20647,12 @@
       <c r="I6" s="174"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="277" t="s">
+      <c r="A7" s="282" t="s">
         <v>144</v>
       </c>
       <c r="B7" s="278"/>
       <c r="C7" s="278"/>
-      <c r="D7" s="279"/>
+      <c r="D7" s="283"/>
       <c r="E7" s="174"/>
       <c r="F7" s="174"/>
       <c r="G7" s="174"/>
@@ -20660,20 +20660,20 @@
       <c r="I7" s="174"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="280" t="s">
+      <c r="A8" s="279" t="s">
         <v>121</v>
       </c>
-      <c r="B8" s="281"/>
+      <c r="B8" s="280"/>
       <c r="C8" s="180">
         <v>12</v>
       </c>
       <c r="D8" s="160"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="280" t="s">
+      <c r="A9" s="279" t="s">
         <v>122</v>
       </c>
-      <c r="B9" s="281"/>
+      <c r="B9" s="280"/>
       <c r="C9" s="172">
         <v>17.23883508535382</v>
       </c>
@@ -20682,10 +20682,10 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="280" t="s">
+      <c r="A10" s="279" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="281"/>
+      <c r="B10" s="280"/>
       <c r="C10" s="172">
         <v>6.2526606521323433</v>
       </c>
@@ -20694,10 +20694,10 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="280" t="s">
+      <c r="A11" s="279" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="281"/>
+      <c r="B11" s="280"/>
       <c r="C11" s="172">
         <f>SQRT(SUM(J24:J33))</f>
         <v>0.5738191903701122</v>
@@ -20707,10 +20707,10 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="283" t="s">
+      <c r="A12" s="276" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="284"/>
+      <c r="B12" s="277"/>
       <c r="C12" s="163">
         <v>4</v>
       </c>
@@ -20730,18 +20730,18 @@
       <c r="I13" s="174"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="277" t="s">
+      <c r="A14" s="282" t="s">
         <v>62</v>
       </c>
       <c r="B14" s="278"/>
       <c r="C14" s="278"/>
-      <c r="D14" s="279"/>
+      <c r="D14" s="283"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="280" t="s">
+      <c r="A15" s="279" t="s">
         <v>128</v>
       </c>
-      <c r="B15" s="281"/>
+      <c r="B15" s="280"/>
       <c r="C15" s="159">
         <v>10</v>
       </c>
@@ -20750,10 +20750,10 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="280" t="s">
+      <c r="A16" s="279" t="s">
         <v>130</v>
       </c>
-      <c r="B16" s="281"/>
+      <c r="B16" s="280"/>
       <c r="C16" s="181">
         <v>5800000</v>
       </c>
@@ -20762,10 +20762,10 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="280" t="s">
+      <c r="A17" s="279" t="s">
         <v>132</v>
       </c>
-      <c r="B17" s="281"/>
+      <c r="B17" s="280"/>
       <c r="C17" s="159">
         <f>1.61</f>
         <v>1.61</v>
@@ -20775,10 +20775,10 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="280" t="s">
+      <c r="A18" s="279" t="s">
         <v>133</v>
       </c>
-      <c r="B18" s="281"/>
+      <c r="B18" s="280"/>
       <c r="C18" s="181">
         <f>C16*C17/C10</f>
         <v>1493444.2343061531</v>
@@ -20789,10 +20789,10 @@
       <c r="E18" s="175"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="280" t="s">
+      <c r="A19" s="279" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="281"/>
+      <c r="B19" s="280"/>
       <c r="C19" s="172">
         <f>C18/58000000*100</f>
         <v>2.5749038522519885</v>
@@ -20802,10 +20802,10 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="283" t="s">
+      <c r="A20" s="276" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="284"/>
+      <c r="B20" s="277"/>
       <c r="C20" s="32">
         <f>1/C18*100000000</f>
         <v>66.959313044895524</v>
@@ -22226,13 +22226,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A14:D14"/>
@@ -22249,6 +22242,13 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -24564,27 +24564,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="277" t="s">
+      <c r="A1" s="282" t="s">
         <v>113</v>
       </c>
       <c r="B1" s="278"/>
       <c r="C1" s="278"/>
-      <c r="D1" s="279"/>
+      <c r="D1" s="283"/>
       <c r="F1" s="114"/>
       <c r="G1" s="114"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="280" t="s">
+      <c r="A2" s="279" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="281"/>
-      <c r="C2" s="281"/>
-      <c r="D2" s="282"/>
+      <c r="B2" s="280"/>
+      <c r="C2" s="280"/>
+      <c r="D2" s="284"/>
       <c r="F2" s="27"/>
-      <c r="G2" s="292" t="s">
+      <c r="G2" s="294" t="s">
         <v>100</v>
       </c>
-      <c r="H2" s="293"/>
+      <c r="H2" s="295"/>
       <c r="I2" s="142">
         <v>50.456606666666659</v>
       </c>
@@ -24593,19 +24593,19 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="277" t="s">
+      <c r="A3" s="282" t="s">
         <v>109</v>
       </c>
       <c r="B3" s="278"/>
       <c r="C3" s="278" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="279"/>
+      <c r="D3" s="283"/>
       <c r="F3" s="103"/>
-      <c r="G3" s="294" t="s">
+      <c r="G3" s="296" t="s">
         <v>101</v>
       </c>
-      <c r="H3" s="276"/>
+      <c r="H3" s="281"/>
       <c r="I3" s="144">
         <v>49.705458333333326</v>
       </c>
@@ -24614,19 +24614,19 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="280" t="s">
+      <c r="A4" s="279" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="281"/>
-      <c r="C4" s="281" t="s">
+      <c r="B4" s="280"/>
+      <c r="C4" s="280" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="282"/>
+      <c r="D4" s="284"/>
       <c r="F4" s="103"/>
-      <c r="G4" s="295" t="s">
+      <c r="G4" s="292" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="296"/>
+      <c r="H4" s="293"/>
       <c r="I4" s="146">
         <v>1.5111988874461302</v>
       </c>
@@ -24635,11 +24635,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="283" t="s">
+      <c r="A5" s="276" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="284"/>
-      <c r="C5" s="284" t="s">
+      <c r="B5" s="277"/>
+      <c r="C5" s="277" t="s">
         <v>112</v>
       </c>
       <c r="D5" s="285"/>
@@ -24871,17 +24871,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24910,18 +24910,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="277" t="s">
+      <c r="A1" s="282" t="s">
         <v>113</v>
       </c>
       <c r="B1" s="278"/>
       <c r="C1" s="278"/>
-      <c r="D1" s="279"/>
+      <c r="D1" s="283"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="H1" s="304" t="s">
+      <c r="H1" s="297" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="305"/>
+      <c r="I1" s="298"/>
       <c r="J1" s="114"/>
       <c r="K1" s="114"/>
       <c r="L1" s="5"/>
@@ -24929,23 +24929,23 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="280" t="s">
+      <c r="A2" s="279" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="281"/>
-      <c r="C2" s="281"/>
-      <c r="D2" s="282"/>
+      <c r="B2" s="280"/>
+      <c r="C2" s="280"/>
+      <c r="D2" s="284"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="H2" s="306" t="s">
+      <c r="H2" s="299" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="307"/>
+      <c r="I2" s="300"/>
       <c r="J2" s="27"/>
-      <c r="K2" s="292" t="s">
+      <c r="K2" s="294" t="s">
         <v>100</v>
       </c>
-      <c r="L2" s="293"/>
+      <c r="L2" s="295"/>
       <c r="M2" s="142">
         <v>50.456606666666659</v>
       </c>
@@ -24954,24 +24954,24 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="277" t="s">
+      <c r="A3" s="282" t="s">
         <v>109</v>
       </c>
       <c r="B3" s="278"/>
       <c r="C3" s="278" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="279"/>
+      <c r="D3" s="283"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="H3" s="300" t="s">
+      <c r="H3" s="301" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="301"/>
-      <c r="K3" s="294" t="s">
+      <c r="I3" s="302"/>
+      <c r="K3" s="296" t="s">
         <v>101</v>
       </c>
-      <c r="L3" s="276"/>
+      <c r="L3" s="281"/>
       <c r="M3" s="144">
         <v>49.705458333333326</v>
       </c>
@@ -24980,24 +24980,24 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="280" t="s">
+      <c r="A4" s="279" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="281"/>
-      <c r="C4" s="281" t="s">
+      <c r="B4" s="280"/>
+      <c r="C4" s="280" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="282"/>
+      <c r="D4" s="284"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="H4" s="302" t="s">
+      <c r="H4" s="303" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="303"/>
-      <c r="K4" s="295" t="s">
+      <c r="I4" s="304"/>
+      <c r="K4" s="292" t="s">
         <v>102</v>
       </c>
-      <c r="L4" s="296"/>
+      <c r="L4" s="293"/>
       <c r="M4" s="146">
         <v>1.5111988874461302</v>
       </c>
@@ -25006,11 +25006,11 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="283" t="s">
+      <c r="A5" s="276" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="284"/>
-      <c r="C5" s="284" t="s">
+      <c r="B5" s="277"/>
+      <c r="C5" s="277" t="s">
         <v>112</v>
       </c>
       <c r="D5" s="285"/>
@@ -25033,18 +25033,18 @@
       <c r="B7" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="297" t="s">
+      <c r="C7" s="305" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="298"/>
-      <c r="E7" s="298"/>
-      <c r="F7" s="298"/>
-      <c r="G7" s="297" t="s">
+      <c r="D7" s="306"/>
+      <c r="E7" s="306"/>
+      <c r="F7" s="306"/>
+      <c r="G7" s="305" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="298"/>
-      <c r="I7" s="298"/>
-      <c r="J7" s="299"/>
+      <c r="H7" s="306"/>
+      <c r="I7" s="306"/>
+      <c r="J7" s="307"/>
       <c r="K7" s="100" t="s">
         <v>5</v>
       </c>
@@ -25054,12 +25054,12 @@
       <c r="M7" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="N7" s="297" t="s">
+      <c r="N7" s="305" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="298"/>
-      <c r="P7" s="298"/>
-      <c r="Q7" s="299"/>
+      <c r="O7" s="306"/>
+      <c r="P7" s="306"/>
+      <c r="Q7" s="307"/>
       <c r="R7" s="100" t="s">
         <v>5</v>
       </c>
@@ -28069,11 +28069,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="N7:Q7"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K4:L4"/>
@@ -28082,11 +28082,11 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -28100,7 +28100,7 @@
   </sheetPr>
   <dimension ref="A1:T145"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
@@ -28115,18 +28115,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="277" t="s">
+      <c r="A1" s="282" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="278"/>
       <c r="C1" s="278" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="279"/>
+      <c r="D1" s="283"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="H1" s="312"/>
-      <c r="I1" s="312"/>
+      <c r="H1" s="308"/>
+      <c r="I1" s="308"/>
       <c r="J1" s="114"/>
       <c r="K1" s="114"/>
       <c r="L1" s="5"/>
@@ -28134,20 +28134,20 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="280" t="s">
+      <c r="A2" s="279" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="281"/>
-      <c r="C2" s="281" t="s">
+      <c r="B2" s="280"/>
+      <c r="C2" s="280" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="282"/>
+      <c r="D2" s="284"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="H2" s="313" t="s">
+      <c r="H2" s="309" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="314"/>
+      <c r="I2" s="310"/>
       <c r="J2" s="27"/>
       <c r="K2" s="99"/>
       <c r="L2" s="5"/>
@@ -28155,59 +28155,59 @@
       <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="280" t="s">
+      <c r="A3" s="279" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="281"/>
-      <c r="C3" s="281" t="s">
+      <c r="B3" s="280"/>
+      <c r="C3" s="280" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="282"/>
+      <c r="D3" s="284"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="H3" s="300" t="s">
+      <c r="H3" s="301" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="301"/>
+      <c r="I3" s="302"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="280" t="s">
+      <c r="A4" s="279" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="281"/>
-      <c r="C4" s="281" t="s">
+      <c r="B4" s="280"/>
+      <c r="C4" s="280" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="282"/>
+      <c r="D4" s="284"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="H4" s="310" t="s">
+      <c r="H4" s="311" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="311"/>
+      <c r="I4" s="312"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="283" t="s">
+      <c r="A5" s="276" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="284"/>
-      <c r="C5" s="284" t="s">
+      <c r="B5" s="277"/>
+      <c r="C5" s="277" t="s">
         <v>97</v>
       </c>
       <c r="D5" s="285"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="98"/>
-      <c r="H5" s="308" t="s">
+      <c r="H5" s="313" t="s">
         <v>163</v>
       </c>
-      <c r="I5" s="309"/>
+      <c r="I5" s="314"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
@@ -28225,18 +28225,18 @@
       <c r="B7" s="166" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="297" t="s">
+      <c r="C7" s="305" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="298"/>
-      <c r="E7" s="298"/>
-      <c r="F7" s="298"/>
-      <c r="G7" s="297" t="s">
+      <c r="D7" s="306"/>
+      <c r="E7" s="306"/>
+      <c r="F7" s="306"/>
+      <c r="G7" s="305" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="298"/>
-      <c r="I7" s="298"/>
-      <c r="J7" s="299"/>
+      <c r="H7" s="306"/>
+      <c r="I7" s="306"/>
+      <c r="J7" s="307"/>
       <c r="K7" s="165" t="s">
         <v>5</v>
       </c>
@@ -28246,12 +28246,12 @@
       <c r="M7" s="166" t="s">
         <v>52</v>
       </c>
-      <c r="N7" s="297" t="s">
+      <c r="N7" s="305" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="298"/>
-      <c r="P7" s="298"/>
-      <c r="Q7" s="299"/>
+      <c r="O7" s="306"/>
+      <c r="P7" s="306"/>
+      <c r="Q7" s="307"/>
       <c r="R7" s="165" t="s">
         <v>5</v>
       </c>
@@ -31610,24 +31610,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31657,87 +31657,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="277" t="s">
+      <c r="A1" s="282" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="278"/>
       <c r="C1" s="278" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="279"/>
+      <c r="D1" s="283"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="H1" s="312"/>
-      <c r="I1" s="312"/>
+      <c r="H1" s="308"/>
+      <c r="I1" s="308"/>
       <c r="J1" s="114"/>
       <c r="K1" s="114"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="280" t="s">
+      <c r="A2" s="279" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="281"/>
-      <c r="C2" s="281" t="s">
+      <c r="B2" s="280"/>
+      <c r="C2" s="280" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="282"/>
+      <c r="D2" s="284"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="H2" s="313" t="s">
+      <c r="H2" s="309" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="314"/>
+      <c r="I2" s="310"/>
       <c r="J2" s="27"/>
       <c r="K2" s="93"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="280" t="s">
+      <c r="A3" s="279" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="281"/>
-      <c r="C3" s="281" t="s">
+      <c r="B3" s="280"/>
+      <c r="C3" s="280" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="282"/>
+      <c r="D3" s="284"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="H3" s="300" t="s">
+      <c r="H3" s="301" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="301"/>
+      <c r="I3" s="302"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="280" t="s">
+      <c r="A4" s="279" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="281"/>
-      <c r="C4" s="281" t="s">
+      <c r="B4" s="280"/>
+      <c r="C4" s="280" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="282"/>
+      <c r="D4" s="284"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="H4" s="310" t="s">
+      <c r="H4" s="311" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="311"/>
+      <c r="I4" s="312"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="283" t="s">
+      <c r="A5" s="276" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="284"/>
-      <c r="C5" s="284" t="s">
+      <c r="B5" s="277"/>
+      <c r="C5" s="277" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="285"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="98"/>
-      <c r="H5" s="308" t="s">
+      <c r="H5" s="313" t="s">
         <v>163</v>
       </c>
-      <c r="I5" s="309"/>
+      <c r="I5" s="314"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
@@ -31747,11 +31747,11 @@
       <c r="D6" s="5"/>
       <c r="F6" s="98"/>
       <c r="G6" s="98"/>
-      <c r="V6" s="277" t="s">
+      <c r="V6" s="282" t="s">
         <v>120</v>
       </c>
       <c r="W6" s="278"/>
-      <c r="X6" s="279"/>
+      <c r="X6" s="283"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="94" t="s">
@@ -31760,18 +31760,18 @@
       <c r="B7" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="297" t="s">
+      <c r="C7" s="305" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="298"/>
-      <c r="E7" s="298"/>
-      <c r="F7" s="298"/>
-      <c r="G7" s="297" t="s">
+      <c r="D7" s="306"/>
+      <c r="E7" s="306"/>
+      <c r="F7" s="306"/>
+      <c r="G7" s="305" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="298"/>
-      <c r="I7" s="298"/>
-      <c r="J7" s="299"/>
+      <c r="H7" s="306"/>
+      <c r="I7" s="306"/>
+      <c r="J7" s="307"/>
       <c r="K7" s="94" t="s">
         <v>5</v>
       </c>
@@ -31781,12 +31781,12 @@
       <c r="M7" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="N7" s="297" t="s">
+      <c r="N7" s="305" t="s">
         <v>60</v>
       </c>
-      <c r="O7" s="298"/>
-      <c r="P7" s="298"/>
-      <c r="Q7" s="299"/>
+      <c r="O7" s="306"/>
+      <c r="P7" s="306"/>
+      <c r="Q7" s="307"/>
       <c r="R7" s="94" t="s">
         <v>5</v>
       </c>
@@ -35216,12 +35216,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="V6:X6"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="G7:J7"/>
     <mergeCell ref="A3:B3"/>
@@ -35230,11 +35229,12 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -35248,7 +35248,7 @@
   </sheetPr>
   <dimension ref="A1:X178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8:J8"/>
     </sheetView>
   </sheetViews>
@@ -35263,32 +35263,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="317" t="s">
+      <c r="A1" s="322" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="318"/>
-      <c r="C1" s="318"/>
-      <c r="D1" s="318"/>
-      <c r="E1" s="319"/>
-      <c r="H1" s="312"/>
-      <c r="I1" s="312"/>
-      <c r="K1" s="315" t="s">
+      <c r="B1" s="323"/>
+      <c r="C1" s="323"/>
+      <c r="D1" s="323"/>
+      <c r="E1" s="324"/>
+      <c r="H1" s="308"/>
+      <c r="I1" s="308"/>
+      <c r="K1" s="320" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="316"/>
+      <c r="L1" s="321"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="320" t="s">
+      <c r="A2" s="325" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="321"/>
-      <c r="C2" s="321"/>
-      <c r="D2" s="321"/>
-      <c r="E2" s="322"/>
-      <c r="H2" s="313" t="s">
+      <c r="B2" s="326"/>
+      <c r="C2" s="326"/>
+      <c r="D2" s="326"/>
+      <c r="E2" s="327"/>
+      <c r="H2" s="309" t="s">
         <v>68</v>
       </c>
-      <c r="I2" s="314"/>
+      <c r="I2" s="310"/>
       <c r="K2" s="104" t="s">
         <v>72</v>
       </c>
@@ -35297,17 +35297,17 @@
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="325" t="s">
+      <c r="A3" s="315" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="326"/>
-      <c r="C3" s="326"/>
-      <c r="D3" s="326"/>
-      <c r="E3" s="327"/>
-      <c r="H3" s="300" t="s">
+      <c r="B3" s="316"/>
+      <c r="C3" s="316"/>
+      <c r="D3" s="316"/>
+      <c r="E3" s="317"/>
+      <c r="H3" s="301" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="301"/>
+      <c r="I3" s="302"/>
       <c r="K3" s="107" t="s">
         <v>73</v>
       </c>
@@ -35323,15 +35323,15 @@
         <f>0.06</f>
         <v>0.06</v>
       </c>
-      <c r="C4" s="328" t="s">
+      <c r="C4" s="318" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="328"/>
-      <c r="E4" s="329"/>
-      <c r="H4" s="310" t="s">
+      <c r="D4" s="318"/>
+      <c r="E4" s="319"/>
+      <c r="H4" s="311" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="311"/>
+      <c r="I4" s="312"/>
       <c r="K4" s="104" t="s">
         <v>71</v>
       </c>
@@ -35346,15 +35346,15 @@
       <c r="B5" s="68">
         <v>1.9400000000000001E-2</v>
       </c>
-      <c r="C5" s="323" t="s">
+      <c r="C5" s="328" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="323"/>
-      <c r="E5" s="324"/>
-      <c r="H5" s="308" t="s">
+      <c r="D5" s="328"/>
+      <c r="E5" s="329"/>
+      <c r="H5" s="313" t="s">
         <v>163</v>
       </c>
-      <c r="I5" s="309"/>
+      <c r="I5" s="314"/>
       <c r="K5" s="106">
         <v>150</v>
       </c>
@@ -35413,18 +35413,18 @@
       <c r="B8" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="297" t="s">
+      <c r="C8" s="305" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="298"/>
-      <c r="E8" s="298"/>
-      <c r="F8" s="298"/>
-      <c r="G8" s="297" t="s">
+      <c r="D8" s="306"/>
+      <c r="E8" s="306"/>
+      <c r="F8" s="306"/>
+      <c r="G8" s="305" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="298"/>
-      <c r="I8" s="298"/>
-      <c r="J8" s="298"/>
+      <c r="H8" s="306"/>
+      <c r="I8" s="306"/>
+      <c r="J8" s="306"/>
       <c r="K8" s="100" t="s">
         <v>5</v>
       </c>
@@ -35956,19 +35956,19 @@
       <c r="B21" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="297" t="s">
+      <c r="C21" s="305" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="298"/>
-      <c r="E21" s="298"/>
-      <c r="F21" s="298"/>
-      <c r="G21" s="297" t="str">
+      <c r="D21" s="306"/>
+      <c r="E21" s="306"/>
+      <c r="F21" s="306"/>
+      <c r="G21" s="305" t="str">
         <f>"  average relative permeability (1-10)"</f>
         <v xml:space="preserve">  average relative permeability (1-10)</v>
       </c>
-      <c r="H21" s="298"/>
-      <c r="I21" s="298"/>
-      <c r="J21" s="298"/>
+      <c r="H21" s="306"/>
+      <c r="I21" s="306"/>
+      <c r="J21" s="306"/>
       <c r="K21" s="100" t="s">
         <v>5</v>
       </c>
@@ -37869,6 +37869,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="C21:F21"/>
@@ -37878,12 +37884,6 @@
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>